<commit_message>
Optimized methods for HomeOversUnders -
</commit_message>
<xml_diff>
--- a/streaks.xlsx
+++ b/streaks.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HomeOver0" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HomeConceedBelow3" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,79 +441,79 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>HomeOver0</t>
+          <t>HomeConceedBelow3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Inter</t>
+          <t>RBLeipzig</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Atl.Madrid</t>
+          <t>Sekhukhune</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>ShakhtarDonetsk</t>
+          <t>Inter</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Cardiff</t>
+          <t>Lens</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>AstonVilla</t>
+          <t>GreutherFurth</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Magdeburg</t>
+          <t>Atl.Madrid</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -526,72 +526,72 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Sevilla</t>
+          <t>ShakhtarDonetsk</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>BayerLeverkusen</t>
+          <t>Aarhus</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Brighton</t>
+          <t>Cardiff</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Barcelona</t>
+          <t>GoldenArrows</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Bochum</t>
+          <t>AstonVilla</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Lille</t>
+          <t>Feyenoord</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -604,85 +604,85 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Rennes</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Ipswich</t>
+          <t>Lazio</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>PSV</t>
+          <t>Ch.Odessa</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Arsenal</t>
+          <t>Odense</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Juventus</t>
+          <t>Coventry</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Twente</t>
+          <t>BayerLeverkusen</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -695,20 +695,20 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Paderborn</t>
+          <t>RichardsBay</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Brondby</t>
+          <t>Brighton</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -721,7 +721,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Fiorentina</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -734,33 +734,33 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Wehen</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C24" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Wolves</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>FKZorya</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -773,46 +773,46 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Tottenham</t>
+          <t>Midtjylland</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C27" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Nijmegen</t>
+          <t>Hull</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C28" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Frosinone</t>
+          <t>Bochum</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Villarreal</t>
+          <t>ChippaUtd.</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -825,33 +825,33 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Nottingham</t>
+          <t>Lille</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C31" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Toulouse</t>
+          <t>Liverpool</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>HamburgerSV</t>
+          <t>Udinese</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -864,130 +864,1508 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Rotherham</t>
+          <t>HerthaBerlin</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C34" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>RealMadrid</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C35" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Newcastle</t>
+          <t>Kryvbas</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C36" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Vejle</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C37" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Brentford</t>
+          <t>KaizerChiefs</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C38" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Nurnberg</t>
+          <t>PSV</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C39" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Dusseldorf</t>
+          <t>Napoli</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>ManchesterCity</t>
+          <t>Metz</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C41" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>AZAlkmaar</t>
+          <t>WestHam</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C42" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
+          <t>FCCopenhagen</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>8</v>
+      </c>
+      <c r="C43" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>Leeds</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>8</v>
+      </c>
+      <c r="C44" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>BayernMunich</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>6</v>
+      </c>
+      <c r="C45" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>Polokwane</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>7</v>
+      </c>
+      <c r="C46" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>Monza</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>6</v>
+      </c>
+      <c r="C47" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>LeHavre</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>6</v>
+      </c>
+      <c r="C48" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>Vitesse</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>6</v>
+      </c>
+      <c r="C49" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>Zhytomyr</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>6</v>
+      </c>
+      <c r="C50" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>Silkeborg</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>8</v>
+      </c>
+      <c r="C51" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>Middlesbrough</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>8</v>
+      </c>
+      <c r="C52" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>CapeTown</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>10</v>
+      </c>
+      <c r="C53" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>7</v>
+      </c>
+      <c r="C54" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>Reims</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>6</v>
+      </c>
+      <c r="C55" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>6</v>
+      </c>
+      <c r="C56" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>Twente</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>6</v>
+      </c>
+      <c r="C57" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>Paderborn</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>6</v>
+      </c>
+      <c r="C58" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>Almeria</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>7</v>
+      </c>
+      <c r="C59" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>Brondby</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>7</v>
+      </c>
+      <c r="C60" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>Stuttgart</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>6</v>
+      </c>
+      <c r="C61" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>Montpellier</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>5</v>
+      </c>
+      <c r="C62" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>CrystalPalace</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>6</v>
+      </c>
+      <c r="C63" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>Schalke</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>6</v>
+      </c>
+      <c r="C64" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>KolosKovalivka</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>8</v>
+      </c>
+      <c r="C65" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>Nice</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>6</v>
+      </c>
+      <c r="C66" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>B.Monchengladbach</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>6</v>
+      </c>
+      <c r="C67" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>Sittard</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>6</v>
+      </c>
+      <c r="C68" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>ManchesterUtd</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>7</v>
+      </c>
+      <c r="C69" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>RukhLviv</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>9</v>
+      </c>
+      <c r="C70" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>St.Pauli</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>7</v>
+      </c>
+      <c r="C71" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>AthBilbao</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>7</v>
+      </c>
+      <c r="C72" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>6</v>
+      </c>
+      <c r="C73" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>Swallows</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>6</v>
+      </c>
+      <c r="C74" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>Hannover</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>6</v>
+      </c>
+      <c r="C75" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>Getafe</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>6</v>
+      </c>
+      <c r="C76" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>Sassuolo</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>7</v>
+      </c>
+      <c r="C77" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>Dnipro-1</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>7</v>
+      </c>
+      <c r="C78" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>Nordsjaelland</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>7</v>
+      </c>
+      <c r="C79" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>Watford</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>9</v>
+      </c>
+      <c r="C80" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>Wolfsburg</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>5</v>
+      </c>
+      <c r="C81" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>Nantes</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>6</v>
+      </c>
+      <c r="C82" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>6</v>
+      </c>
+      <c r="C83" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>HansaRostock</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>7</v>
+      </c>
+      <c r="C84" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>Viborg</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>7</v>
+      </c>
+      <c r="C85" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>Strasbourg</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>6</v>
+      </c>
+      <c r="C86" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>5</v>
+      </c>
+      <c r="C87" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>Frosinone</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>6</v>
+      </c>
+      <c r="C88" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>OrlandoPirates</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>5</v>
+      </c>
+      <c r="C89" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>KarlsruherSC</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>6</v>
+      </c>
+      <c r="C90" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>Lyngby</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>7</v>
+      </c>
+      <c r="C91" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>FCKoln</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>5</v>
+      </c>
+      <c r="C92" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>Zwolle</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>6</v>
+      </c>
+      <c r="C93" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>Nottingham</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>5</v>
+      </c>
+      <c r="C94" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>Toulouse</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>5</v>
+      </c>
+      <c r="C95" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>RoyalAM</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>5</v>
+      </c>
+      <c r="C96" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>HamburgerSV</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>6</v>
+      </c>
+      <c r="C97" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>6</v>
+      </c>
+      <c r="C98" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>Rotherham</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>8</v>
+      </c>
+      <c r="C99" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>Metalist1925</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>6</v>
+      </c>
+      <c r="C100" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>6</v>
+      </c>
+      <c r="C101" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>ASRoma</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>6</v>
+      </c>
+      <c r="C102" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>Stellenbosch</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>6</v>
+      </c>
+      <c r="C103" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>Kaiserslautern</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>7</v>
+      </c>
+      <c r="C104" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>Alaves</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>6</v>
+      </c>
+      <c r="C105" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>8</v>
+      </c>
+      <c r="C106" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>Hoffenheim</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>5</v>
+      </c>
+      <c r="C107" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>6</v>
+      </c>
+      <c r="C108" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>G.A.Eagles</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>6</v>
+      </c>
+      <c r="C109" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>Marseille</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>5</v>
+      </c>
+      <c r="C110" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>Nurnberg</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>6</v>
+      </c>
+      <c r="C111" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>RealSociedad</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>7</v>
+      </c>
+      <c r="C112" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>Birmingham</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>8</v>
+      </c>
+      <c r="C113" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t>Mainz</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>5</v>
+      </c>
+      <c r="C114" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>Lorient</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>6</v>
+      </c>
+      <c r="C115" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t>Verona</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>5</v>
+      </c>
+      <c r="C116" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>VfLOsnabruck</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>7</v>
+      </c>
+      <c r="C117" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>CeltaVigo</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>7</v>
+      </c>
+      <c r="C118" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>Dyn.Kyiv</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>5</v>
+      </c>
+      <c r="C119" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="inlineStr">
+        <is>
+          <t>BristolCity</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>8</v>
+      </c>
+      <c r="C120" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>TSGalaxy</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>6</v>
+      </c>
+      <c r="C121" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>UnionBerlin</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>5</v>
+      </c>
+      <c r="C122" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>6</v>
+      </c>
+      <c r="C123" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>6</v>
+      </c>
+      <c r="C124" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t>ACMilan</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>5</v>
+      </c>
+      <c r="C125" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="inlineStr">
+        <is>
+          <t>Dusseldorf</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>7</v>
+      </c>
+      <c r="C126" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>Betis</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>6</v>
+      </c>
+      <c r="C127" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="inlineStr">
+        <is>
+          <t>ManchesterCity</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>5</v>
+      </c>
+      <c r="C128" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>5</v>
+      </c>
+      <c r="C129" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="inlineStr">
+        <is>
+          <t>Millwall</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>8</v>
+      </c>
+      <c r="C130" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="inlineStr">
+        <is>
+          <t>LasPalmas</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>6</v>
+      </c>
+      <c r="C131" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="inlineStr">
+        <is>
+          <t>Plymouth</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>8</v>
+      </c>
+      <c r="C132" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>6</v>
+      </c>
+      <c r="C133" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>5</v>
+      </c>
+      <c r="C134" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="inlineStr">
+        <is>
+          <t>EintrachtFrankfurt</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>5</v>
+      </c>
+      <c r="C135" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="inlineStr">
+        <is>
+          <t>SupersportUtd</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>5</v>
+      </c>
+      <c r="C136" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="inlineStr">
+        <is>
+          <t>Brest</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>5</v>
+      </c>
+      <c r="C137" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="inlineStr">
+        <is>
+          <t>Empoli</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>6</v>
+      </c>
+      <c r="C138" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="inlineStr">
+        <is>
+          <t>Stoke</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>8</v>
+      </c>
+      <c r="C139" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="inlineStr">
+        <is>
+          <t>Swansea</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>8</v>
+      </c>
+      <c r="C140" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="inlineStr">
+        <is>
+          <t>AmaZulu</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>5</v>
+      </c>
+      <c r="C141" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="inlineStr">
+        <is>
+          <t>WestBrom</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>8</v>
+      </c>
+      <c r="C142" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="inlineStr">
+        <is>
+          <t>CadizCF</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>6</v>
+      </c>
+      <c r="C143" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="inlineStr">
+        <is>
+          <t>Leicester</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>8</v>
+      </c>
+      <c r="C144" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="inlineStr">
+        <is>
+          <t>Heerenveen</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>5</v>
+      </c>
+      <c r="C145" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="inlineStr">
+        <is>
+          <t>Mallorca</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>5</v>
+      </c>
+      <c r="C146" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="inlineStr">
+        <is>
+          <t>Girona</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>6</v>
+      </c>
+      <c r="C147" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="inlineStr">
+        <is>
+          <t>AZAlkmaar</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>5</v>
+      </c>
+      <c r="C148" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="inlineStr">
+        <is>
           <t>MamelodiSundowns</t>
         </is>
       </c>
-      <c r="B43" t="n">
+      <c r="B149" t="n">
         <v>3</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C149" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
From Seaonal to FullTimeOvers rewrite
</commit_message>
<xml_diff>
--- a/streaks.xlsx
+++ b/streaks.xlsx
@@ -11,6 +11,15 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayFullTimeOver2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayBTS" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayGoal" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayUnder3Goal" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayUnder4Goal" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayUnderFirstHlvGoal" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayUnderFirstHlv1Goal" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayUnderFirstHlv2Goal" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayOverFirstHlvGoal" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayOverFirstHlv1Goal" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayOverFirstHlv2Goal" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AwayConceedSecHlvGoal" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,209 +460,359 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Walsall</t>
+          <t>WestHam</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Brighton</t>
+          <t>Liverpool</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>FeralpiSalo</t>
+          <t>SheffieldUtd</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Mansfield</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>OxfordUtd</t>
+          <t>Brighton</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Newport</t>
+          <t>Bournemouth</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Ternana</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>9</v>
-      </c>
-      <c r="C8" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>AwayGamesPlayed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AwayOverFirstHlvGoal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>Bournemouth</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>11</v>
-      </c>
-      <c r="C9" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Sutton</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Middlesbrough</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>11</v>
-      </c>
-      <c r="C11" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Norwich</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>StockportCounty</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>10</v>
-      </c>
-      <c r="C13" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>SheffieldUtd</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>9</v>
-      </c>
-      <c r="C14" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="B5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>AwayGamesPlayed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AwayOverFirstHlv1Goal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>AwayGamesPlayed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AwayOverFirstHlv2Goal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>AwayGamesPlayed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AwayConceedSecHlvGoal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>WestHam</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>9</v>
-      </c>
-      <c r="C15" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Liverpool</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>9</v>
-      </c>
-      <c r="C16" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="B2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>Newcastle</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="B4" t="n">
         <v>4</v>
       </c>
-      <c r="C17" t="n">
-        <v>4</v>
+      <c r="C4" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -667,7 +826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -690,7 +849,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Ternana</t>
+          <t>WestHam</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -703,66 +862,27 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Bournemouth</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Middlesbrough</t>
+          <t>Bournemouth</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Norwich</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>11</v>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>WestHam</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>9</v>
-      </c>
-      <c r="C6" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Newcastle</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -776,7 +896,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -799,7 +919,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Ternana</t>
+          <t>WestHam</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -812,33 +932,33 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Norwich</t>
+          <t>Liverpool</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>StockportCounty</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>WestHam</t>
+          <t>Brighton</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -846,32 +966,6 @@
       </c>
       <c r="C5" t="n">
         <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Liverpool</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>9</v>
-      </c>
-      <c r="C6" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Newcastle</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -885,7 +979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -908,72 +1002,72 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Genk</t>
+          <t>WestHam</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Westerlo</t>
+          <t>CrystalPalace</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>RoyaleUnion</t>
+          <t>Tottenham</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Mansfield</t>
+          <t>Liverpool</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Southampton</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Ternana</t>
+          <t>Brighton</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -986,24 +1080,146 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Peterborough</t>
+          <t>Bournemouth</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" t="n">
-        <v>11</v>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>AwayGamesPlayed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AwayUnder3Goal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Nottingham</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>WestHam</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>CrystalPalace</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>AstonVilla</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Anderlecht</t>
+          <t>Wolves</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="n">
         <v>9</v>
@@ -1012,7 +1228,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Parma</t>
+          <t>Brentford</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1025,46 +1241,46 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Leicester</t>
+          <t>SheffieldUtd</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Cittadella</t>
+          <t>Burnley</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Bournemouth</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Sampdoria</t>
+          <t>ManchesterUtd</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1072,81 +1288,842 @@
       </c>
       <c r="C14" t="n">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>AwayGamesPlayed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AwayUnder4Goal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>ManchesterCity</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Nottingham</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>WestHam</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>CrystalPalace</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>AstonVilla</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Wolves</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>8</v>
+      </c>
+      <c r="C12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>SheffieldUtd</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>9</v>
+      </c>
+      <c r="C13" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Burnley</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>9</v>
+      </c>
+      <c r="C14" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Sudtirol</t>
+          <t>Newcastle</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Middlesbrough</t>
+          <t>Everton</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Norwich</t>
+          <t>ManchesterUtd</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Crewe</t>
+          <t>Brighton</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>StockportCounty</t>
+          <t>Bournemouth</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" t="n">
-        <v>10</v>
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>AwayGamesPlayed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AwayUnderFirstHlvGoal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Wolves</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>SheffieldUtd</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>AwayGamesPlayed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AwayUnderFirstHlv1Goal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Nottingham</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>WestHam</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>CrystalPalace</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>AstonVilla</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Wolves</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>SheffieldUtd</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Burnley</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>9</v>
+      </c>
+      <c r="C13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>ManchesterUtd</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>9</v>
+      </c>
+      <c r="C14" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Brighton</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>9</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>9</v>
+      </c>
+      <c r="C17" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>AwayGamesPlayed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AwayUnderFirstHlv2Goal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>ManchesterCity</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Nottingham</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>WestHam</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>CrystalPalace</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>AstonVilla</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Wolves</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>8</v>
+      </c>
+      <c r="C12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>SheffieldUtd</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>9</v>
+      </c>
+      <c r="C13" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Burnley</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>9</v>
+      </c>
+      <c r="C14" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>ManchesterUtd</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>9</v>
+      </c>
+      <c r="C17" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Brighton</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>9</v>
+      </c>
+      <c r="C18" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>9</v>
+      </c>
+      <c r="C19" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Derby</t>
+          <t>Arsenal</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" t="n">
         <v>9</v>
@@ -1155,92 +2132,14 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Barnsley</t>
+          <t>Chelsea</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="n">
         <v>9</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Swansea</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>11</v>
-      </c>
-      <c r="C22" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>CrystalPalace</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>9</v>
-      </c>
-      <c r="C23" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Tottenham</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>9</v>
-      </c>
-      <c r="C24" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>WestHam</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>9</v>
-      </c>
-      <c r="C25" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>Liverpool</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>9</v>
-      </c>
-      <c r="C26" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>Newcastle</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>4</v>
-      </c>
-      <c r="C27" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>